<commit_message>
kart be kart hamid podr mehdi
</commit_message>
<xml_diff>
--- a/SWIFT.xlsx
+++ b/SWIFT.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>معدن</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>چنگال</t>
+  </si>
+  <si>
+    <t>پود ماشین + کارت به کارت حمید</t>
   </si>
 </sst>
 </file>
@@ -410,13 +413,13 @@
   <dimension ref="A1:O1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M1" sqref="A1:M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
     <col min="11" max="11" width="10.42578125" customWidth="1"/>
   </cols>
@@ -582,6 +585,17 @@
         <v>-6.8</v>
       </c>
     </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <v>-41.1</v>
+      </c>
+    </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>12</v>
@@ -600,7 +614,7 @@
       </c>
       <c r="E23" s="1">
         <f t="shared" ref="E23:M23" si="0">SUM(E1:E22)</f>
-        <v>-6.5</v>
+        <v>-4.5</v>
       </c>
       <c r="F23" s="1">
         <f t="shared" si="0"/>
@@ -616,7 +630,7 @@
       </c>
       <c r="I23" s="1">
         <f t="shared" si="0"/>
-        <v>41.1</v>
+        <v>0</v>
       </c>
       <c r="J23" s="1">
         <f t="shared" si="0"/>
@@ -636,7 +650,7 @@
       </c>
       <c r="O23" s="1">
         <f>SUM(B23:M23)*-1</f>
-        <v>26.999999999999996</v>
+        <v>66.099999999999994</v>
       </c>
     </row>
     <row r="1048576" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
sobhane barbary+ sobhane barbar+tokhme morgh
</commit_message>
<xml_diff>
--- a/SWIFT.xlsx
+++ b/SWIFT.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>معدن</t>
   </si>
@@ -79,6 +79,18 @@
   </si>
   <si>
     <t>پود ماشین + کارت به کارت حمید</t>
+  </si>
+  <si>
+    <t>سالاد ماکارونی</t>
+  </si>
+  <si>
+    <t>خشتی</t>
+  </si>
+  <si>
+    <t>بربری صبحانه   4.5</t>
+  </si>
+  <si>
+    <t>صبحانه تخم مرغ بربری   11.5</t>
   </si>
 </sst>
 </file>
@@ -414,7 +426,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K9" sqref="K9"/>
+      <selection pane="bottomLeft" activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,6 +476,9 @@
       <c r="M1" t="s">
         <v>11</v>
       </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B2">
@@ -597,6 +612,9 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
       <c r="C9">
         <v>-3</v>
       </c>
@@ -611,6 +629,37 @@
       </c>
       <c r="J9">
         <v>-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10">
+        <v>3.375</v>
+      </c>
+      <c r="L10">
+        <v>1.125</v>
+      </c>
+      <c r="N10">
+        <v>1.125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11">
+        <v>-2.2999999999999998</v>
+      </c>
+      <c r="E11">
+        <v>-2.2999999999999998</v>
+      </c>
+      <c r="K11">
+        <v>-2.2999999999999998</v>
+      </c>
+      <c r="M11">
+        <v>-2.2999999999999998</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -623,15 +672,15 @@
       </c>
       <c r="C23" s="1">
         <f>SUM(C2:C17)</f>
-        <v>-19.400000000000002</v>
+        <v>-18.325000000000003</v>
       </c>
       <c r="D23" s="1">
         <f>SUM(D1:D22)</f>
         <v>8.1999999999999993</v>
       </c>
       <c r="E23" s="1">
-        <f t="shared" ref="E23:M23" si="0">SUM(E1:E22)</f>
-        <v>-7.5</v>
+        <f t="shared" ref="E23:N23" si="0">SUM(E1:E22)</f>
+        <v>-9.8000000000000007</v>
       </c>
       <c r="F23" s="1">
         <f t="shared" si="0"/>
@@ -655,19 +704,23 @@
       </c>
       <c r="K23" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-2.2999999999999998</v>
       </c>
       <c r="L23" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.125</v>
       </c>
       <c r="M23" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-2.2999999999999998</v>
+      </c>
+      <c r="N23" s="1">
+        <f t="shared" si="0"/>
+        <v>1.125</v>
       </c>
       <c r="O23" s="1">
         <f>SUM(B23:M23)*-1</f>
-        <v>63.099999999999994</v>
+        <v>67.8</v>
       </c>
     </row>
     <row r="1048576" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
tasviye mehdi kart be kart
</commit_message>
<xml_diff>
--- a/SWIFT.xlsx
+++ b/SWIFT.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>معدن</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>صبحانه تخم مرغ بربری   11.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">کارت به کارت مهدی </t>
   </si>
 </sst>
 </file>
@@ -426,7 +429,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M12" sqref="M12"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,6 +665,14 @@
         <v>-2.2999999999999998</v>
       </c>
     </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12">
+        <v>18.324999999999999</v>
+      </c>
+    </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>12</v>
@@ -672,7 +683,7 @@
       </c>
       <c r="C23" s="1">
         <f>SUM(C2:C17)</f>
-        <v>-18.325000000000003</v>
+        <v>0</v>
       </c>
       <c r="D23" s="1">
         <f>SUM(D1:D22)</f>
@@ -720,7 +731,7 @@
       </c>
       <c r="O23" s="1">
         <f>SUM(B23:M23)*-1</f>
-        <v>67.8</v>
+        <v>49.474999999999994</v>
       </c>
     </row>
     <row r="1048576" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
kart be karte soheil ravabet mehdi-soheil
</commit_message>
<xml_diff>
--- a/SWIFT.xlsx
+++ b/SWIFT.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>معدن</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t xml:space="preserve">کارت به کارت مهدی </t>
+  </si>
+  <si>
+    <t>کارت به کارت به سهیل</t>
+  </si>
+  <si>
+    <t>روابط فی مابین مهدی و سهیل</t>
   </si>
 </sst>
 </file>
@@ -428,8 +434,8 @@
   <dimension ref="A1:O1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N1" sqref="A1:N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,7 +497,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>11.7</v>
+        <v>40</v>
       </c>
       <c r="E2">
         <v>4</v>
@@ -673,13 +679,32 @@
         <v>18.324999999999999</v>
       </c>
     </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13">
+        <v>-36.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14">
+        <v>7.5</v>
+      </c>
+      <c r="D14">
+        <v>-7.5</v>
+      </c>
+    </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B23" s="1">
         <f>SUM(B2:B17)</f>
-        <v>-5</v>
+        <v>2.5</v>
       </c>
       <c r="C23" s="1">
         <f>SUM(C2:C17)</f>
@@ -687,7 +712,7 @@
       </c>
       <c r="D23" s="1">
         <f>SUM(D1:D22)</f>
-        <v>8.1999999999999993</v>
+        <v>-7.5</v>
       </c>
       <c r="E23" s="1">
         <f t="shared" ref="E23:N23" si="0">SUM(E1:E22)</f>
@@ -731,13 +756,13 @@
       </c>
       <c r="O23" s="1">
         <f>SUM(B23:M23)*-1</f>
-        <v>49.474999999999994</v>
+        <v>57.674999999999997</v>
       </c>
     </row>
     <row r="1048576" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B1048576">
         <f>SUM(B2:B1048575)</f>
-        <v>-10</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sobhane eshgh shame feragh roghn
</commit_message>
<xml_diff>
--- a/SWIFT.xlsx
+++ b/SWIFT.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>معدن</t>
   </si>
@@ -112,6 +112,18 @@
   </si>
   <si>
     <t>تسویه خشتی و سلیمانی</t>
+  </si>
+  <si>
+    <t>کیک نوید</t>
+  </si>
+  <si>
+    <t>صبحانه در محضر عشق</t>
+  </si>
+  <si>
+    <t>شام شب فراغ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">روغن </t>
   </si>
 </sst>
 </file>
@@ -447,7 +459,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N23" sqref="A1:N23"/>
+      <selection pane="bottomLeft" activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,7 +756,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -764,7 +776,7 @@
         <v>-1.3</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -775,7 +787,10 @@
         <v>2.2749999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
       <c r="B19">
         <v>-5.75</v>
       </c>
@@ -795,71 +810,137 @@
         <v>-5.75</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20">
+        <v>-2.25</v>
+      </c>
+      <c r="E20">
+        <v>-2.25</v>
+      </c>
+      <c r="H20">
+        <v>-2.25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21">
+        <v>-2.1</v>
+      </c>
+      <c r="I21">
+        <v>8.4</v>
+      </c>
+      <c r="K21">
+        <v>-2.1</v>
+      </c>
+      <c r="N21">
+        <v>-2.1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22">
+        <v>-0.63</v>
+      </c>
+      <c r="C22">
+        <v>-0.63</v>
+      </c>
+      <c r="D22">
+        <v>-0.63</v>
+      </c>
+      <c r="F22">
+        <v>-0.63</v>
+      </c>
+      <c r="G22">
+        <v>-0.63</v>
+      </c>
+      <c r="I22">
+        <v>6.3</v>
+      </c>
+      <c r="J22">
+        <v>-0.63</v>
+      </c>
+      <c r="K22">
+        <v>-0.63</v>
+      </c>
+      <c r="L22">
+        <v>-0.63</v>
+      </c>
+      <c r="N22">
+        <v>-0.63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="1">
-        <f>SUM(B1:B22)</f>
-        <v>3.8499999999999996</v>
-      </c>
-      <c r="C23" s="1">
-        <f t="shared" ref="C23:N23" si="0">SUM(C1:C22)</f>
-        <v>-7.0500000000000034</v>
-      </c>
-      <c r="D23" s="1">
-        <f t="shared" si="0"/>
-        <v>-16.950000000000003</v>
-      </c>
-      <c r="E23" s="1">
-        <f t="shared" si="0"/>
-        <v>24.7</v>
-      </c>
-      <c r="F23" s="1">
-        <f t="shared" si="0"/>
-        <v>-12.95</v>
-      </c>
-      <c r="G23" s="1">
-        <f t="shared" si="0"/>
-        <v>-3</v>
-      </c>
-      <c r="H23" s="1">
-        <f t="shared" si="0"/>
-        <v>-1.8</v>
-      </c>
-      <c r="I23" s="1">
-        <f t="shared" si="0"/>
-        <v>-3</v>
-      </c>
-      <c r="J23" s="1">
-        <f t="shared" si="0"/>
-        <v>-32.75</v>
-      </c>
-      <c r="K23" s="1">
-        <f t="shared" si="0"/>
-        <v>-4.6999999999999993</v>
-      </c>
-      <c r="L23" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M23" s="1">
+      <c r="B34" s="1">
+        <f>SUM(B1:B33)</f>
+        <v>3.2199999999999998</v>
+      </c>
+      <c r="C34" s="1">
+        <f t="shared" ref="C34:N34" si="0">SUM(C1:C33)</f>
+        <v>-9.930000000000005</v>
+      </c>
+      <c r="D34" s="1">
+        <f t="shared" si="0"/>
+        <v>-17.580000000000002</v>
+      </c>
+      <c r="E34" s="1">
+        <f t="shared" si="0"/>
+        <v>20.349999999999998</v>
+      </c>
+      <c r="F34" s="1">
+        <f t="shared" si="0"/>
+        <v>-13.58</v>
+      </c>
+      <c r="G34" s="1">
+        <f t="shared" si="0"/>
+        <v>-3.63</v>
+      </c>
+      <c r="H34" s="1">
+        <f t="shared" si="0"/>
+        <v>-4.05</v>
+      </c>
+      <c r="I34" s="1">
+        <f t="shared" si="0"/>
+        <v>11.7</v>
+      </c>
+      <c r="J34" s="1">
+        <f t="shared" si="0"/>
+        <v>-33.380000000000003</v>
+      </c>
+      <c r="K34" s="1">
+        <f t="shared" si="0"/>
+        <v>-7.4299999999999988</v>
+      </c>
+      <c r="L34" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.63</v>
+      </c>
+      <c r="M34" s="1">
         <f t="shared" si="0"/>
         <v>-2.2999999999999998</v>
       </c>
-      <c r="N23" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O23" s="1">
-        <f>SUM(B23:M23)*-1</f>
-        <v>55.95</v>
+      <c r="N34" s="1">
+        <f t="shared" si="0"/>
+        <v>-2.73</v>
+      </c>
+      <c r="O34" s="1">
+        <f>SUM(B34:M34)*-1</f>
+        <v>57.240000000000009</v>
       </c>
     </row>
     <row r="1048576" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B1048576">
         <f>SUM(B2:B1048575)</f>
-        <v>7.6999999999999993</v>
+        <v>6.4399999999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sandevich koh estakhr ravabet fi ma beyn soheil pasha
</commit_message>
<xml_diff>
--- a/SWIFT.xlsx
+++ b/SWIFT.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>معدن</t>
   </si>
@@ -124,6 +124,18 @@
   </si>
   <si>
     <t xml:space="preserve">روغن </t>
+  </si>
+  <si>
+    <t>کوه سه شنبه</t>
+  </si>
+  <si>
+    <t>ساندویچ</t>
+  </si>
+  <si>
+    <t>روابط فی مابین سهیل و پاشا</t>
+  </si>
+  <si>
+    <t>استخر</t>
   </si>
 </sst>
 </file>
@@ -458,8 +470,8 @@
   <dimension ref="A1:O1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M33" sqref="M33"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,7 +530,7 @@
         <v>0.9</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>9.93</v>
       </c>
       <c r="D2">
         <v>40</v>
@@ -876,6 +888,65 @@
         <v>-0.63</v>
       </c>
     </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23">
+        <v>-3</v>
+      </c>
+      <c r="D23">
+        <v>10</v>
+      </c>
+      <c r="E23">
+        <v>-4</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24">
+        <v>-1.5</v>
+      </c>
+      <c r="F24">
+        <v>-1.5</v>
+      </c>
+      <c r="H24">
+        <v>-1.5</v>
+      </c>
+      <c r="I24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25">
+        <v>7</v>
+      </c>
+      <c r="F25">
+        <v>-3.5</v>
+      </c>
+      <c r="K25">
+        <v>-3.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26">
+        <v>-10</v>
+      </c>
+      <c r="F26">
+        <v>10</v>
+      </c>
+    </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>12</v>
@@ -886,19 +957,19 @@
       </c>
       <c r="C34" s="1">
         <f t="shared" ref="C34:N34" si="0">SUM(C1:C33)</f>
-        <v>-9.930000000000005</v>
+        <v>-3.0000000000000009</v>
       </c>
       <c r="D34" s="1">
         <f t="shared" si="0"/>
-        <v>-17.580000000000002</v>
+        <v>-7.5800000000000018</v>
       </c>
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>20.349999999999998</v>
+        <v>11.849999999999998</v>
       </c>
       <c r="F34" s="1">
         <f t="shared" si="0"/>
-        <v>-13.58</v>
+        <v>-8.5799999999999983</v>
       </c>
       <c r="G34" s="1">
         <f t="shared" si="0"/>
@@ -906,11 +977,11 @@
       </c>
       <c r="H34" s="1">
         <f t="shared" si="0"/>
-        <v>-4.05</v>
+        <v>-5.55</v>
       </c>
       <c r="I34" s="1">
         <f t="shared" si="0"/>
-        <v>11.7</v>
+        <v>18.7</v>
       </c>
       <c r="J34" s="1">
         <f t="shared" si="0"/>
@@ -918,7 +989,7 @@
       </c>
       <c r="K34" s="1">
         <f t="shared" si="0"/>
-        <v>-7.4299999999999988</v>
+        <v>-10.93</v>
       </c>
       <c r="L34" s="1">
         <f t="shared" si="0"/>
@@ -934,7 +1005,7 @@
       </c>
       <c r="O34" s="1">
         <f>SUM(B34:M34)*-1</f>
-        <v>57.240000000000009</v>
+        <v>41.810000000000009</v>
       </c>
     </row>
     <row r="1048576" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
sandevich-estakhr-koh-ravabete fimabein pasha-soheil-tasviye mahmud
</commit_message>
<xml_diff>
--- a/SWIFT.xlsx
+++ b/SWIFT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>معدن</t>
   </si>
@@ -126,16 +126,19 @@
     <t xml:space="preserve">روغن </t>
   </si>
   <si>
-    <t>کوه سه شنبه</t>
-  </si>
-  <si>
     <t>ساندویچ</t>
   </si>
   <si>
-    <t>روابط فی مابین سهیل و پاشا</t>
-  </si>
-  <si>
     <t>استخر</t>
+  </si>
+  <si>
+    <t>کوه</t>
+  </si>
+  <si>
+    <t>روابط فی مابین پاشا و سهیل</t>
+  </si>
+  <si>
+    <t>تسویه محمود</t>
   </si>
 </sst>
 </file>
@@ -151,7 +154,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -170,6 +173,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -183,10 +192,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,8 +480,8 @@
   <dimension ref="A1:O1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K25" sqref="K25"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N34" sqref="A1:N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,43 +495,43 @@
       <c r="A1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -530,7 +540,7 @@
         <v>0.9</v>
       </c>
       <c r="C2">
-        <v>9.93</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>40</v>
@@ -892,22 +902,19 @@
       <c r="A23" t="s">
         <v>35</v>
       </c>
-      <c r="C23">
-        <v>-3</v>
-      </c>
       <c r="D23">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E23">
-        <v>-4</v>
-      </c>
-      <c r="I23">
-        <v>1</v>
+        <v>-3.5</v>
+      </c>
+      <c r="K23">
+        <v>-3.5</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E24">
         <v>-1.5</v>
@@ -924,27 +931,38 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="C25">
+        <v>-3</v>
+      </c>
+      <c r="D25">
+        <v>10</v>
       </c>
       <c r="E25">
-        <v>7</v>
-      </c>
-      <c r="F25">
-        <v>-3.5</v>
-      </c>
-      <c r="K25">
-        <v>-3.5</v>
+        <v>-4</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="D26">
+        <v>-10</v>
       </c>
       <c r="E26">
-        <v>-10</v>
-      </c>
-      <c r="F26">
         <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="J27">
+        <v>33.380000000000003</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
@@ -957,19 +975,19 @@
       </c>
       <c r="C34" s="1">
         <f t="shared" ref="C34:N34" si="0">SUM(C1:C33)</f>
-        <v>-3.0000000000000009</v>
+        <v>-12.930000000000005</v>
       </c>
       <c r="D34" s="1">
         <f t="shared" si="0"/>
-        <v>-7.5800000000000018</v>
+        <v>-10.580000000000002</v>
       </c>
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>11.849999999999998</v>
+        <v>21.349999999999998</v>
       </c>
       <c r="F34" s="1">
         <f t="shared" si="0"/>
-        <v>-8.5799999999999983</v>
+        <v>-15.08</v>
       </c>
       <c r="G34" s="1">
         <f t="shared" si="0"/>
@@ -985,7 +1003,7 @@
       </c>
       <c r="J34" s="1">
         <f t="shared" si="0"/>
-        <v>-33.380000000000003</v>
+        <v>0</v>
       </c>
       <c r="K34" s="1">
         <f t="shared" si="0"/>
@@ -1005,7 +1023,7 @@
       </c>
       <c r="O34" s="1">
         <f>SUM(B34:M34)*-1</f>
-        <v>41.810000000000009</v>
+        <v>18.36000000000001</v>
       </c>
     </row>
     <row r="1048576" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
chay mahmud fimabeyn pasha mahmud
</commit_message>
<xml_diff>
--- a/SWIFT.xlsx
+++ b/SWIFT.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>معدن</t>
   </si>
@@ -139,6 +139,12 @@
   </si>
   <si>
     <t>تسویه محمود</t>
+  </si>
+  <si>
+    <t>چای</t>
+  </si>
+  <si>
+    <t>فیمابین محمود پاشا شاژر</t>
   </si>
 </sst>
 </file>
@@ -480,14 +486,14 @@
   <dimension ref="A1:O1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N34" sqref="A1:N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" customWidth="1"/>
     <col min="11" max="11" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -965,6 +971,37 @@
         <v>33.380000000000003</v>
       </c>
     </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28">
+        <v>-2.4</v>
+      </c>
+      <c r="E28">
+        <v>12</v>
+      </c>
+      <c r="F28">
+        <v>-2.4</v>
+      </c>
+      <c r="I28">
+        <v>-2.4</v>
+      </c>
+      <c r="J28">
+        <v>-2.4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29">
+        <v>-10</v>
+      </c>
+      <c r="J29">
+        <v>10</v>
+      </c>
+    </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>12</v>
@@ -979,15 +1016,15 @@
       </c>
       <c r="D34" s="1">
         <f t="shared" si="0"/>
-        <v>-10.580000000000002</v>
+        <v>-12.980000000000002</v>
       </c>
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>21.349999999999998</v>
+        <v>23.349999999999994</v>
       </c>
       <c r="F34" s="1">
         <f t="shared" si="0"/>
-        <v>-15.08</v>
+        <v>-17.48</v>
       </c>
       <c r="G34" s="1">
         <f t="shared" si="0"/>
@@ -999,11 +1036,11 @@
       </c>
       <c r="I34" s="1">
         <f t="shared" si="0"/>
-        <v>18.7</v>
+        <v>16.3</v>
       </c>
       <c r="J34" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7.6</v>
       </c>
       <c r="K34" s="1">
         <f t="shared" si="0"/>
@@ -1023,7 +1060,7 @@
       </c>
       <c r="O34" s="1">
         <f>SUM(B34:M34)*-1</f>
-        <v>18.36000000000001</v>
+        <v>15.960000000000012</v>
       </c>
     </row>
     <row r="1048576" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
tasviye mehdi esraf+shame mehdi esraf
</commit_message>
<xml_diff>
--- a/SWIFT.xlsx
+++ b/SWIFT.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>معدن</t>
   </si>
@@ -145,6 +145,12 @@
   </si>
   <si>
     <t>فیمابین محمود پاشا شاژر</t>
+  </si>
+  <si>
+    <t>تسویه مهدی اسراف</t>
+  </si>
+  <si>
+    <t>شام مهدی اسراف</t>
   </si>
 </sst>
 </file>
@@ -486,8 +492,8 @@
   <dimension ref="A1:O1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N34" sqref="A1:N34"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1002,6 +1008,34 @@
         <v>10</v>
       </c>
     </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30">
+        <v>9.93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31">
+        <v>12.16</v>
+      </c>
+      <c r="D31">
+        <v>-3.04</v>
+      </c>
+      <c r="E31">
+        <v>-3.04</v>
+      </c>
+      <c r="F31">
+        <v>-3.04</v>
+      </c>
+      <c r="I31">
+        <v>-3.04</v>
+      </c>
+    </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>12</v>
@@ -1012,19 +1046,19 @@
       </c>
       <c r="C34" s="1">
         <f t="shared" ref="C34:N34" si="0">SUM(C1:C33)</f>
-        <v>-12.930000000000005</v>
+        <v>9.1599999999999948</v>
       </c>
       <c r="D34" s="1">
         <f t="shared" si="0"/>
-        <v>-12.980000000000002</v>
+        <v>-16.020000000000003</v>
       </c>
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>23.349999999999994</v>
+        <v>20.309999999999995</v>
       </c>
       <c r="F34" s="1">
         <f t="shared" si="0"/>
-        <v>-17.48</v>
+        <v>-20.52</v>
       </c>
       <c r="G34" s="1">
         <f t="shared" si="0"/>
@@ -1036,7 +1070,7 @@
       </c>
       <c r="I34" s="1">
         <f t="shared" si="0"/>
-        <v>16.3</v>
+        <v>13.260000000000002</v>
       </c>
       <c r="J34" s="1">
         <f t="shared" si="0"/>
@@ -1060,7 +1094,7 @@
       </c>
       <c r="O34" s="1">
         <f>SUM(B34:M34)*-1</f>
-        <v>15.960000000000012</v>
+        <v>6.03000000000001</v>
       </c>
     </row>
     <row r="1048576" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>